<commit_message>
22/11/2022 - 13h55 - MCD StagiairesAFPA Fait
</commit_message>
<xml_diff>
--- a/Exercices/01 - Persistance des données/03 - Remplir les tableaux/02 - Voitures/Marque Modele.xlsx
+++ b/Exercices/01 - Persistance des données/03 - Remplir les tableaux/02 - Voitures/Marque Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\01 - Persistance des données\03 - Remplir les tableaux\02 - Voitures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165C27-8284-4AED-B682-DAC886E78CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD301AE1-1E55-4D61-B1D7-201719E5DEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D748779-E7B7-4DAD-A32C-61751D1BDC23}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="417">
   <si>
     <t>libelle</t>
   </si>
@@ -1287,9 +1287,6 @@
   </si>
   <si>
     <t>idModele</t>
-  </si>
-  <si>
-    <t>=RANDBETWEEN(DATE(2019, 1, 1),DATE(2019, 10, 20))</t>
   </si>
 </sst>
 </file>
@@ -1653,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD4F30C-C795-490F-8B55-EB8148B63D7B}">
   <dimension ref="A1:O426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,20 +1727,20 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="str">
-        <f ca="1">TEXT(DATE(RANDBETWEEN(2020,2022),RANDBETWEEN(1,12),RANDBETWEEN(1,28)),"aaaa-mm-jj")</f>
-        <v>2022-03-23</v>
+        <f ca="1">TEXT(DATE(2020,1,1) + RANDBETWEEN(1,1000),"aaaa-mm-jj")</f>
+        <v>2022-04-12</v>
       </c>
       <c r="M2" t="str">
         <f ca="1">TEXT(EDATE(L2,5),"aaaa-mm-jj")</f>
-        <v>2022-08-23</v>
+        <v>2022-09-12</v>
       </c>
       <c r="N2">
         <f ca="1">RANDBETWEEN($A$2,$A$426)</f>
-        <v>115</v>
+        <v>366</v>
       </c>
       <c r="O2" t="str">
         <f ca="1">"INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("""&amp;L2&amp;""", """&amp;M2&amp;""", "&amp;N2&amp;");"</f>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-23", "2022-08-23", 115);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-04-12", "2022-09-12", 366);</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1778,20 +1775,20 @@
         <v>2</v>
       </c>
       <c r="L3" s="1" t="str">
-        <f ca="1">TEXT(DATE(RANDBETWEEN(2020,2022),RANDBETWEEN(1,12),RANDBETWEEN(1,28)),"aaaa-mm-jj")</f>
-        <v>2022-03-25</v>
+        <f t="shared" ref="L3:L38" ca="1" si="3">TEXT(DATE(2020,1,1) + RANDBETWEEN(1,1000),"aaaa-mm-jj")</f>
+        <v>2021-11-17</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M38" ca="1" si="3">TEXT(EDATE(L3,5),"aaaa-mm-jj")</f>
-        <v>2022-08-25</v>
+        <f t="shared" ref="M3:M38" ca="1" si="4">TEXT(EDATE(L3,5),"aaaa-mm-jj")</f>
+        <v>2022-04-17</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N38" ca="1" si="4">RANDBETWEEN($A$2,$A$426)</f>
-        <v>82</v>
+        <f t="shared" ref="N3:N38" ca="1" si="5">RANDBETWEEN($A$2,$A$426)</f>
+        <v>77</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O38" ca="1" si="5">"INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("""&amp;L3&amp;""", """&amp;M3&amp;""", "&amp;N3&amp;");"</f>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-25", "2022-08-25", 82);</v>
+        <f t="shared" ref="O3:O38" ca="1" si="6">"INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("""&amp;L3&amp;""", """&amp;M3&amp;""", "&amp;N3&amp;");"</f>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-11-17", "2022-04-17", 77);</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1826,20 +1823,20 @@
         <v>3</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f t="shared" ref="L3:L38" ca="1" si="6">TEXT(DATE(RANDBETWEEN(2020,2022),RANDBETWEEN(1,12),RANDBETWEEN(1,28)),"aaaa-mm-jj")</f>
-        <v>2022-12-08</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-03-18</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-05-08</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-08-18</v>
       </c>
       <c r="N4">
-        <f t="shared" ca="1" si="4"/>
-        <v>275</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>213</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-12-08", "2023-05-08", 275);</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-03-18", "2020-08-18", 213);</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1874,20 +1871,20 @@
         <v>4</v>
       </c>
       <c r="L5" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-10-30</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-03-30</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="O5" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-03-13</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-08-13</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ca="1" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-13", "2022-08-13", 20);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-10-30", "2022-03-30", 78);</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1922,20 +1919,20 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-06-20</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-11-20</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="5"/>
+        <v>119</v>
+      </c>
+      <c r="O6" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2021-01-21</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-06-21</v>
-      </c>
-      <c r="N6">
-        <f t="shared" ca="1" si="4"/>
-        <v>219</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-01-21", "2021-06-21", 219);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-06-20", "2022-11-20", 119);</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1970,20 +1967,20 @@
         <v>6</v>
       </c>
       <c r="L7" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-09-19</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-02-19</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="5"/>
+        <v>236</v>
+      </c>
+      <c r="O7" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-05-11</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-10-11</v>
-      </c>
-      <c r="N7">
-        <f t="shared" ca="1" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-05-11", "2022-10-11", 19);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-09-19", "2022-02-19", 236);</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2018,20 +2015,20 @@
         <v>7</v>
       </c>
       <c r="L8" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-02-25</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-07-25</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="5"/>
+        <v>374</v>
+      </c>
+      <c r="O8" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2021-03-08</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-08-08</v>
-      </c>
-      <c r="N8">
-        <f t="shared" ca="1" si="4"/>
-        <v>231</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-03-08", "2021-08-08", 231);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-02-25", "2022-07-25", 374);</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2066,20 +2063,20 @@
         <v>8</v>
       </c>
       <c r="L9" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-02-20</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-07-20</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="5"/>
+        <v>271</v>
+      </c>
+      <c r="O9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-02-28</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-07-28</v>
-      </c>
-      <c r="N9">
-        <f t="shared" ca="1" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-02-28", "2020-07-28", 16);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-02-20", "2021-07-20", 271);</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2114,20 +2111,20 @@
         <v>9</v>
       </c>
       <c r="L10" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-10-23</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-03-23</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="O10" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-09-01</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-02-01</v>
-      </c>
-      <c r="N10">
-        <f t="shared" ca="1" si="4"/>
-        <v>147</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-09-01", "2023-02-01", 147);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-10-23", "2021-03-23", 208);</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2162,20 +2159,20 @@
         <v>10</v>
       </c>
       <c r="L11" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-07-12</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-12-12</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="5"/>
+        <v>370</v>
+      </c>
+      <c r="O11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-01-11</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-06-11</v>
-      </c>
-      <c r="N11">
-        <f t="shared" ca="1" si="4"/>
-        <v>319</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-01-11", "2022-06-11", 319);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-07-12", "2020-12-12", 370);</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2210,20 +2207,20 @@
         <v>11</v>
       </c>
       <c r="L12" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-03-24</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-08-24</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="O12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2021-10-16</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-03-16</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ca="1" si="4"/>
-        <v>181</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-10-16", "2022-03-16", 181);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-24", "2022-08-24", 186);</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2258,20 +2255,20 @@
         <v>12</v>
       </c>
       <c r="L13" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-05-04</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-10-04</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="O13" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-02-25</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-07-25</v>
-      </c>
-      <c r="N13">
-        <f t="shared" ca="1" si="4"/>
-        <v>155</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-02-25", "2020-07-25", 155);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-05-04", "2020-10-04", 82);</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2306,20 +2303,20 @@
         <v>13</v>
       </c>
       <c r="L14" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-03-20</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-08-20</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="5"/>
+        <v>317</v>
+      </c>
+      <c r="O14" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-05-08</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-10-08</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ca="1" si="4"/>
-        <v>205</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-05-08", "2020-10-08", 205);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-03-20", "2020-08-20", 317);</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2354,20 +2351,20 @@
         <v>14</v>
       </c>
       <c r="L15" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-02-11</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-07-11</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="O15" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-03-02</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-08-02</v>
-      </c>
-      <c r="N15">
-        <f t="shared" ca="1" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-03-02", "2020-08-02", 5);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-02-11", "2022-07-11", 26);</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2402,20 +2399,20 @@
         <v>15</v>
       </c>
       <c r="L16" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-10-28</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-03-28</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="5"/>
+        <v>190</v>
+      </c>
+      <c r="O16" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-11-11</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-04-11</v>
-      </c>
-      <c r="N16">
-        <f t="shared" ca="1" si="4"/>
-        <v>155</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-11-11", "2023-04-11", 155);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-10-28", "2021-03-28", 190);</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2450,20 +2447,20 @@
         <v>16</v>
       </c>
       <c r="L17" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-03-14</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-08-14</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="5"/>
+        <v>352</v>
+      </c>
+      <c r="O17" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-08-02</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-01-02</v>
-      </c>
-      <c r="N17">
-        <f t="shared" ca="1" si="4"/>
-        <v>185</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-08-02", "2021-01-02", 185);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-14", "2022-08-14", 352);</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2498,20 +2495,20 @@
         <v>17</v>
       </c>
       <c r="L18" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-04-17</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-09-17</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="O18" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-08-04</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-01-04</v>
-      </c>
-      <c r="N18">
-        <f t="shared" ca="1" si="4"/>
-        <v>336</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-08-04", "2021-01-04", 336);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-04-17", "2020-09-17", 325);</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2546,20 +2543,20 @@
         <v>18</v>
       </c>
       <c r="L19" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-04-04</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-09-04</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="5"/>
+        <v>386</v>
+      </c>
+      <c r="O19" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-12-04</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-05-04</v>
-      </c>
-      <c r="N19">
-        <f t="shared" ca="1" si="4"/>
-        <v>83</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-12-04", "2021-05-04", 83);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-04-04", "2020-09-04", 386);</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2594,20 +2591,20 @@
         <v>19</v>
       </c>
       <c r="L20" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-01-27</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-06-27</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="5"/>
+        <v>119</v>
+      </c>
+      <c r="O20" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-06-04</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-11-04</v>
-      </c>
-      <c r="N20">
-        <f t="shared" ca="1" si="4"/>
-        <v>137</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-06-04", "2020-11-04", 137);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-01-27", "2021-06-27", 119);</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2642,20 +2639,20 @@
         <v>20</v>
       </c>
       <c r="L21" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-09-10</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-02-10</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="5"/>
+        <v>259</v>
+      </c>
+      <c r="O21" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-12-26</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-05-26</v>
-      </c>
-      <c r="N21">
-        <f t="shared" ca="1" si="4"/>
-        <v>390</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-12-26", "2023-05-26", 390);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-09-10", "2022-02-10", 259);</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2690,20 +2687,20 @@
         <v>21</v>
       </c>
       <c r="L22" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-02-16</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-07-16</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="5"/>
+        <v>382</v>
+      </c>
+      <c r="O22" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-11-01</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-04-01</v>
-      </c>
-      <c r="N22">
-        <f t="shared" ca="1" si="4"/>
-        <v>198</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-11-01", "2023-04-01", 198);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-02-16", "2020-07-16", 382);</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2738,20 +2735,20 @@
         <v>22</v>
       </c>
       <c r="L23" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-05-17</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-10-17</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="5"/>
+        <v>341</v>
+      </c>
+      <c r="O23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2021-07-21</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-12-21</v>
-      </c>
-      <c r="N23">
-        <f t="shared" ca="1" si="4"/>
-        <v>105</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-07-21", "2021-12-21", 105);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-05-17", "2021-10-17", 341);</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2786,20 +2783,20 @@
         <v>23</v>
       </c>
       <c r="L24" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-08-26</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2023-01-26</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="5"/>
+        <v>268</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-03-03</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-08-03</v>
-      </c>
-      <c r="N24">
-        <f t="shared" ca="1" si="4"/>
-        <v>308</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-03-03", "2020-08-03", 308);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-08-26", "2023-01-26", 268);</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2834,20 +2831,20 @@
         <v>24</v>
       </c>
       <c r="L25" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-06-07</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-11-07</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-12-07</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-05-07</v>
-      </c>
-      <c r="N25">
-        <f t="shared" ca="1" si="4"/>
-        <v>131</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-12-07", "2023-05-07", 131);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-06-07", "2021-11-07", 11);</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2882,20 +2879,20 @@
         <v>25</v>
       </c>
       <c r="L26" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-10-01</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-03-01</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="5"/>
+        <v>219</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-02-09</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-07-09</v>
-      </c>
-      <c r="N26">
-        <f t="shared" ca="1" si="4"/>
-        <v>269</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-02-09", "2022-07-09", 269);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-10-01", "2022-03-01", 219);</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2930,20 +2927,20 @@
         <v>26</v>
       </c>
       <c r="L27" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-08-17</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-01-17</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="5"/>
+        <v>409</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-11-28</v>
-      </c>
-      <c r="M27" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-04-28</v>
-      </c>
-      <c r="N27">
-        <f t="shared" ca="1" si="4"/>
-        <v>81</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-11-28", "2023-04-28", 81);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-08-17", "2022-01-17", 409);</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2978,20 +2975,20 @@
         <v>27</v>
       </c>
       <c r="L28" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-04-02</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-09-02</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="O28" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-03-07</v>
-      </c>
-      <c r="M28" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-08-07</v>
-      </c>
-      <c r="N28">
-        <f t="shared" ca="1" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-07", "2022-08-07", 100);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-04-02", "2022-09-02", 186);</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3026,20 +3023,20 @@
         <v>28</v>
       </c>
       <c r="L29" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-09-17</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-02-17</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="5"/>
+        <v>274</v>
+      </c>
+      <c r="O29" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-08-21</v>
-      </c>
-      <c r="M29" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-01-21</v>
-      </c>
-      <c r="N29">
-        <f t="shared" ca="1" si="4"/>
-        <v>172</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-08-21", "2021-01-21", 172);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-09-17", "2022-02-17", 274);</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3074,20 +3071,20 @@
         <v>29</v>
       </c>
       <c r="L30" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-12-16</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-05-16</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="5"/>
+        <v>358</v>
+      </c>
+      <c r="O30" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-09-16</v>
-      </c>
-      <c r="M30" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-02-16</v>
-      </c>
-      <c r="N30">
-        <f t="shared" ca="1" si="4"/>
-        <v>128</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-09-16", "2023-02-16", 128);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-12-16", "2021-05-16", 358);</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3122,20 +3119,20 @@
         <v>30</v>
       </c>
       <c r="L31" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-06-01</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-11-01</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="5"/>
+        <v>214</v>
+      </c>
+      <c r="O31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-05-24</v>
-      </c>
-      <c r="M31" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-10-24</v>
-      </c>
-      <c r="N31">
-        <f t="shared" ca="1" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-05-24", "2022-10-24", 70);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-06-01", "2022-11-01", 214);</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3170,20 +3167,20 @@
         <v>31</v>
       </c>
       <c r="L32" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-09-14</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-02-14</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="5"/>
+        <v>199</v>
+      </c>
+      <c r="O32" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2021-04-10</v>
-      </c>
-      <c r="M32" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2021-09-10</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ca="1" si="4"/>
-        <v>357</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-04-10", "2021-09-10", 357);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-09-14", "2021-02-14", 199);</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3218,20 +3215,20 @@
         <v>32</v>
       </c>
       <c r="L33" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-03-04</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-08-04</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O33" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-04-26</v>
-      </c>
-      <c r="M33" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-09-26</v>
-      </c>
-      <c r="N33">
-        <f t="shared" ca="1" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="O33" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-04-26", "2022-09-26", 26);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-03-04", "2021-08-04", 6);</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3266,20 +3263,20 @@
         <v>33</v>
       </c>
       <c r="L34" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-08-28</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-01-28</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="5"/>
+        <v>209</v>
+      </c>
+      <c r="O34" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-07-10</v>
-      </c>
-      <c r="M34" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-12-10</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ca="1" si="4"/>
-        <v>149</v>
-      </c>
-      <c r="O34" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-07-10", "2022-12-10", 149);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-08-28", "2021-01-28", 209);</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3314,20 +3311,20 @@
         <v>34</v>
       </c>
       <c r="L35" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-08-20</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2023-01-20</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="5"/>
+        <v>283</v>
+      </c>
+      <c r="O35" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-02-07</v>
-      </c>
-      <c r="M35" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-07-07</v>
-      </c>
-      <c r="N35">
-        <f t="shared" ca="1" si="4"/>
-        <v>292</v>
-      </c>
-      <c r="O35" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-02-07", "2020-07-07", 292);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-08-20", "2023-01-20", 283);</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3362,20 +3359,20 @@
         <v>35</v>
       </c>
       <c r="L36" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2020-01-03</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020-06-03</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="5"/>
+        <v>399</v>
+      </c>
+      <c r="O36" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-06-10</v>
-      </c>
-      <c r="M36" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2022-11-10</v>
-      </c>
-      <c r="N36">
-        <f t="shared" ca="1" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="O36" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-06-10", "2022-11-10", 24);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-01-03", "2020-06-03", 399);</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3410,20 +3407,20 @@
         <v>36</v>
       </c>
       <c r="L37" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2022-03-04</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2022-08-04</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="5"/>
+        <v>407</v>
+      </c>
+      <c r="O37" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2022-08-12</v>
-      </c>
-      <c r="M37" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2023-01-12</v>
-      </c>
-      <c r="N37">
-        <f t="shared" ca="1" si="4"/>
-        <v>245</v>
-      </c>
-      <c r="O37" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-08-12", "2023-01-12", 245);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2022-03-04", "2022-08-04", 407);</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3458,20 +3455,20 @@
         <v>37</v>
       </c>
       <c r="L38" s="1" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>2021-01-15</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2021-06-15</v>
+      </c>
+      <c r="N38">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="O38" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2020-06-03</v>
-      </c>
-      <c r="M38" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>2020-11-03</v>
-      </c>
-      <c r="N38">
-        <f t="shared" ca="1" si="4"/>
-        <v>408</v>
-      </c>
-      <c r="O38" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2020-06-03", "2020-11-03", 408);</v>
+        <v>INSERT INTO Commandes (dateCommande,dateLivraison,idModele) VALUES ("2021-01-15", "2021-06-15", 12);</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3704,9 +3701,6 @@
         <f t="shared" si="1"/>
         <v>INSERT INTO Modeles (libelle, idMarque) VALUES ("430", 4);</v>
       </c>
-      <c r="O47" t="s">
-        <v>417</v>
-      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -3726,10 +3720,6 @@
         <f t="shared" si="1"/>
         <v>INSERT INTO Modeles (libelle, idMarque) VALUES ("435", 4);</v>
       </c>
-      <c r="O48" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(DATE(2020,1,1),TODAY()),"aaaa-mm-jj")</f>
-        <v>2022-09-28</v>
-      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -3769,10 +3759,7 @@
         <f t="shared" si="1"/>
         <v>INSERT INTO Modeles (libelle, idMarque) VALUES ("520", 4);</v>
       </c>
-      <c r="N50" s="1">
-        <f ca="1">TODAY()</f>
-        <v>44887</v>
-      </c>
+      <c r="N50" s="1"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">

</xml_diff>